<commit_message>
alt: Fill all the data that are missing in fluxo.csv
</commit_message>
<xml_diff>
--- a/app/fluxo.xlsx
+++ b/app/fluxo.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="207">
   <si>
     <t xml:space="preserve">FLUXO DE CAIXA</t>
   </si>
@@ -109,52 +109,52 @@
     <t xml:space="preserve">RESULTADO</t>
   </si>
   <si>
-    <t xml:space="preserve">Receita Exames</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Receita Anestesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Receitas Consulta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESAS TOTAIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA COM ANESTESIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA TIM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA ALUGUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA ENERGIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA INTERNET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA COM CRMV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA REMÉDIOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA COM ALIMENTAÇÃO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA COM COMBUSTÍVEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA COM PÓS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA COM PLANO DE SAÚDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESA COM LAZER</t>
+    <t xml:space="preserve">ReceitaExames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReceitaAnestesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReceitasConsulta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESASTOTAIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESACOMANESTESIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESATIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESAALUGUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESAENERGIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESAINTERNET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESACOMCRMV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESAREMEDIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESACOMALIMENTACAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESACOMCOMBUSTIVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESACOMPOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESACOMPLANODESAUDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESACOMLAZER</t>
   </si>
   <si>
     <t xml:space="preserve">IMPOSTO</t>
@@ -166,40 +166,43 @@
     <t xml:space="preserve">INVESTIMENTO</t>
   </si>
   <si>
+    <t xml:space="preserve">LUCRO/PREJUIZO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METAS RECEITAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECEITAS REALIZADAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIF %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METAS DESPESAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESAS REALIZADAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METAS DE RESULTADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METAS RESULTADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESULTADO REALIZADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despesas</t>
+  </si>
+  <si>
     <t xml:space="preserve">LUCRO / PREJUÍZO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METAS RECEITAS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RECEITAS REALIZADAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIF %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METAS DESPESAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESPESAS REALIZADAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METAS DE RESULTADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METAS RESULTADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESULTADO REALIZADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Receita</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Despesas</t>
   </si>
   <si>
     <t xml:space="preserve">No mês de Novembro você Obteve um lucro de R$ 15.219,85</t>
@@ -512,7 +515,43 @@
     <t xml:space="preserve">Vendas</t>
   </si>
   <si>
+    <t xml:space="preserve">DESPESA COM ANESTESIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA TIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA ALUGUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA ENERGIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA INTERNET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA COM CRMV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA REMÉDIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA COM ALIMENTAÇÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA COM COMBUSTÍVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA COM PÓS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA COM PLANO DE SAÚDE</t>
+  </si>
+  <si>
     <t xml:space="preserve">FATURAMENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESPESA COM LAZER</t>
   </si>
   <si>
     <t xml:space="preserve">Essa Mês</t>
@@ -2793,11 +2832,11 @@
         </c:ser>
         <c:gapWidth val="65"/>
         <c:overlap val="0"/>
-        <c:axId val="18021387"/>
-        <c:axId val="11004777"/>
+        <c:axId val="54278859"/>
+        <c:axId val="18346271"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18021387"/>
+        <c:axId val="54278859"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2829,7 +2868,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11004777"/>
+        <c:crossAx val="18346271"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2837,7 +2876,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11004777"/>
+        <c:axId val="18346271"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2879,7 +2918,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18021387"/>
+        <c:crossAx val="54278859"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -3038,10 +3077,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Receita Anestesia</c:v>
+                  <c:v>ReceitaAnestesia</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Receitas Consulta</c:v>
+                  <c:v>ReceitasConsulta</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3769,40 +3808,40 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>DESPESA COM ANESTESIA</c:v>
+                  <c:v>DESPESACOMANESTESIA</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>DESPESA TIM</c:v>
+                  <c:v>DESPESATIM</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DESPESA ALUGUEL</c:v>
+                  <c:v>DESPESAALUGUEL</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>DESPESA ENERGIA</c:v>
+                  <c:v>DESPESAENERGIA</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DESPESA INTERNET</c:v>
+                  <c:v>DESPESAINTERNET</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>DESPESA COM CRMV</c:v>
+                  <c:v>DESPESACOMCRMV</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>DESPESA REMÉDIOS</c:v>
+                  <c:v>DESPESAREMEDIOS</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>DESPESA COM ALIMENTAÇÃO</c:v>
+                  <c:v>DESPESACOMALIMENTACAO</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>DESPESA COM COMBUSTÍVEL</c:v>
+                  <c:v>DESPESACOMCOMBUSTIVEL</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>DESPESA COM PÓS</c:v>
+                  <c:v>DESPESACOMPOS</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>DESPESA COM PLANO DE SAÚDE</c:v>
+                  <c:v>DESPESACOMPLANODESAUDE</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>DESPESA COM LAZER</c:v>
+                  <c:v>DESPESACOMLAZER</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>IMPOSTO</c:v>
@@ -3939,10 +3978,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.136043360433604"/>
-          <c:y val="0.0409760972765887"/>
-          <c:w val="0.727913279132791"/>
-          <c:h val="0.641209294578163"/>
+          <c:x val="0.136050734457152"/>
+          <c:y val="0.0409795102448776"/>
+          <c:w val="0.727898531085696"/>
+          <c:h val="0.641179410294853"/>
         </c:manualLayout>
       </c:layout>
       <c:doughnutChart>
@@ -4818,8 +4857,8 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2782136"/>
-        <c:axId val="40438622"/>
+        <c:axId val="14066201"/>
+        <c:axId val="74224455"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4980,11 +5019,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="2782136"/>
-        <c:axId val="40438622"/>
+        <c:axId val="14066201"/>
+        <c:axId val="74224455"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2782136"/>
+        <c:axId val="14066201"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5016,7 +5055,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40438622"/>
+        <c:crossAx val="74224455"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5024,7 +5063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40438622"/>
+        <c:axId val="74224455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5063,7 +5102,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2782136"/>
+        <c:crossAx val="14066201"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5097,9 +5136,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1130400</xdr:colOff>
+      <xdr:colOff>1130040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>736920</xdr:rowOff>
+      <xdr:rowOff>736560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5113,7 +5152,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="1852560" cy="736920"/>
+          <a:ext cx="1852200" cy="736560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5139,9 +5178,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>158400</xdr:colOff>
+      <xdr:colOff>158040</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>127080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5155,7 +5194,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3553200" cy="898920"/>
+          <a:ext cx="3552840" cy="898560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5181,9 +5220,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1130400</xdr:colOff>
+      <xdr:colOff>1130040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>736920</xdr:rowOff>
+      <xdr:rowOff>736560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5197,7 +5236,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="1852560" cy="736920"/>
+          <a:ext cx="1852200" cy="736560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5223,9 +5262,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>304200</xdr:colOff>
+      <xdr:colOff>303840</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5234,7 +5273,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="2862360"/>
-        <a:ext cx="4019040" cy="2299320"/>
+        <a:ext cx="4018680" cy="2298960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5253,9 +5292,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>492120</xdr:colOff>
+      <xdr:colOff>491760</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>190080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5264,7 +5303,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3030840" y="2736000"/>
-        <a:ext cx="3885120" cy="2838600"/>
+        <a:ext cx="3884040" cy="2838240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5283,9 +5322,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1392120</xdr:colOff>
+      <xdr:colOff>1391760</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5294,7 +5333,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2995200" y="2670120"/>
-        <a:ext cx="10032840" cy="2927520"/>
+        <a:ext cx="10031760" cy="2927160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5313,9 +5352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>498960</xdr:colOff>
+      <xdr:colOff>498600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5329,7 +5368,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3482280" cy="896400"/>
+          <a:ext cx="3481920" cy="896040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5355,9 +5394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>189720</xdr:colOff>
+      <xdr:colOff>189360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5367,7 +5406,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7120080" y="1041120"/>
-          <a:ext cx="6968520" cy="4291920"/>
+          <a:ext cx="6968160" cy="4291560"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5407,9 +5446,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>332640</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5418,7 +5457,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7589880" y="982440"/>
-        <a:ext cx="6641640" cy="4322160"/>
+        <a:ext cx="6641280" cy="4321800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5437,9 +5476,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>456840</xdr:colOff>
+      <xdr:colOff>456480</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5449,7 +5488,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="520560" y="1136520"/>
-          <a:ext cx="2862360" cy="1513080"/>
+          <a:ext cx="2862000" cy="1512720"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5489,9 +5528,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>576720</xdr:colOff>
+      <xdr:colOff>576360</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5501,7 +5540,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533160" y="1215360"/>
-          <a:ext cx="775080" cy="365040"/>
+          <a:ext cx="774720" cy="364680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5555,9 +5594,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>108720</xdr:colOff>
+      <xdr:colOff>108360</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5567,7 +5606,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="520560" y="1702800"/>
-          <a:ext cx="1782720" cy="472680"/>
+          <a:ext cx="1782360" cy="472320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5622,9 +5661,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>370800</xdr:colOff>
+      <xdr:colOff>370440</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5634,7 +5673,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2628000" y="1228680"/>
-          <a:ext cx="668880" cy="525960"/>
+          <a:ext cx="668520" cy="525600"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5674,9 +5713,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>313920</xdr:colOff>
+      <xdr:colOff>313560</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>174600</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5696,7 +5735,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2677320" y="1307520"/>
-          <a:ext cx="562680" cy="400680"/>
+          <a:ext cx="562320" cy="400320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5717,9 +5756,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>132840</xdr:colOff>
+      <xdr:colOff>132480</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -5729,9 +5768,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="3838680" y="1140840"/>
-          <a:ext cx="2877840" cy="1513080"/>
+          <a:ext cx="2877480" cy="1512720"/>
           <a:chOff x="3838680" y="1140840"/>
-          <a:chExt cx="2877840" cy="1513080"/>
+          <a:chExt cx="2877480" cy="1512720"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -5742,7 +5781,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3857400" y="1140840"/>
-            <a:ext cx="2859120" cy="1513080"/>
+            <a:ext cx="2858760" cy="1512720"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst>
@@ -5779,7 +5818,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3944880" y="1226520"/>
-            <a:ext cx="1309320" cy="332640"/>
+            <a:ext cx="1308960" cy="332280"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -5830,7 +5869,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="5931720" y="1217160"/>
-            <a:ext cx="659160" cy="525960"/>
+            <a:ext cx="658800" cy="525600"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst>
@@ -5877,7 +5916,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="6005880" y="1264680"/>
-            <a:ext cx="507600" cy="408960"/>
+            <a:ext cx="507240" cy="408600"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -5895,7 +5934,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3838680" y="1655280"/>
-            <a:ext cx="1416240" cy="342000"/>
+            <a:ext cx="1415880" cy="341640"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -5947,7 +5986,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="5352480" y="2347560"/>
-            <a:ext cx="1204200" cy="216720"/>
+            <a:ext cx="1203840" cy="216360"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6002,9 +6041,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>487080</xdr:colOff>
+      <xdr:colOff>486720</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6014,7 +6053,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="550800" y="2964600"/>
-          <a:ext cx="2862360" cy="1513080"/>
+          <a:ext cx="2862000" cy="1512720"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6054,9 +6093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6066,7 +6105,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3857040" y="2958840"/>
-          <a:ext cx="2862360" cy="1513080"/>
+          <a:ext cx="2862000" cy="1512720"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6106,9 +6145,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>31320</xdr:colOff>
+      <xdr:colOff>30960</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6118,7 +6157,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5945760" y="3035160"/>
-          <a:ext cx="669240" cy="525960"/>
+          <a:ext cx="668880" cy="525600"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6158,9 +6197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>513720</xdr:colOff>
+      <xdr:colOff>513360</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>173520</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6174,7 +6213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6071400" y="3095640"/>
-          <a:ext cx="294480" cy="392760"/>
+          <a:ext cx="294120" cy="392400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6195,9 +6234,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6207,7 +6246,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3981600" y="3019320"/>
-          <a:ext cx="1224360" cy="263880"/>
+          <a:ext cx="1224000" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6261,9 +6300,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>336240</xdr:colOff>
+      <xdr:colOff>335880</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6273,7 +6312,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4064040" y="3426120"/>
-          <a:ext cx="1392840" cy="342000"/>
+          <a:ext cx="1392480" cy="341640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6328,9 +6367,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>47880</xdr:colOff>
+      <xdr:colOff>47520</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>83520</xdr:rowOff>
+      <xdr:rowOff>83160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6340,7 +6379,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5263560" y="4057560"/>
-          <a:ext cx="1368000" cy="293040"/>
+          <a:ext cx="1367640" cy="292680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6394,9 +6433,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>14040</xdr:colOff>
+      <xdr:colOff>13680</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>118800</xdr:rowOff>
+      <xdr:rowOff>118440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6406,7 +6445,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2005920" y="2304720"/>
-          <a:ext cx="1665720" cy="300240"/>
+          <a:ext cx="1665360" cy="299880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6460,9 +6499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>125280</xdr:colOff>
+      <xdr:colOff>124920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>97560</xdr:rowOff>
+      <xdr:rowOff>97200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6472,7 +6511,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="585000" y="3047400"/>
-          <a:ext cx="1734840" cy="365040"/>
+          <a:ext cx="1734480" cy="364680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6526,9 +6565,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>370800</xdr:colOff>
+      <xdr:colOff>370440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6538,7 +6577,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2628000" y="3073320"/>
-          <a:ext cx="668880" cy="525960"/>
+          <a:ext cx="668520" cy="525600"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6578,9 +6617,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>317520</xdr:colOff>
+      <xdr:colOff>317160</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6594,7 +6633,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2729160" y="3094560"/>
-          <a:ext cx="514440" cy="414720"/>
+          <a:ext cx="514080" cy="414360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6615,9 +6654,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>185040</xdr:colOff>
+      <xdr:colOff>184680</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6627,7 +6666,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="596880" y="3503160"/>
-          <a:ext cx="1782720" cy="472680"/>
+          <a:ext cx="1782360" cy="472320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6682,9 +6721,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>71280</xdr:colOff>
+      <xdr:colOff>70920</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:rowOff>147240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6694,7 +6733,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2063160" y="4114800"/>
-          <a:ext cx="1665720" cy="299880"/>
+          <a:ext cx="1665360" cy="299520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6748,9 +6787,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>428040</xdr:colOff>
+      <xdr:colOff>427680</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -6760,9 +6799,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="210240" y="4848120"/>
-          <a:ext cx="11190600" cy="3761640"/>
+          <a:ext cx="11190240" cy="3761280"/>
           <a:chOff x="210240" y="4848120"/>
-          <a:chExt cx="11190600" cy="3761640"/>
+          <a:chExt cx="11190240" cy="3761280"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -6773,7 +6812,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="1405080" y="4848120"/>
-            <a:ext cx="2574720" cy="418320"/>
+            <a:ext cx="2574360" cy="417960"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6822,7 +6861,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3393000" y="5334120"/>
-            <a:ext cx="1794960" cy="343800"/>
+            <a:ext cx="1794600" cy="343440"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6873,7 +6912,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="1369800" y="5315040"/>
-            <a:ext cx="1794960" cy="343800"/>
+            <a:ext cx="1794600" cy="343440"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6924,7 +6963,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="1446480" y="5541480"/>
-            <a:ext cx="1950120" cy="542160"/>
+            <a:ext cx="1949760" cy="541800"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6976,7 +7015,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3573000" y="5579640"/>
-            <a:ext cx="1950120" cy="542160"/>
+            <a:ext cx="1949760" cy="541800"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -7027,7 +7066,7 @@
         </xdr:nvGraphicFramePr>
         <xdr:xfrm>
           <a:off x="210240" y="6302160"/>
-          <a:ext cx="11190600" cy="2307600"/>
+          <a:ext cx="11190240" cy="2307240"/>
         </xdr:xfrm>
         <a:graphic>
           <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7043,7 +7082,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="1388880" y="5659200"/>
-            <a:ext cx="136800" cy="119880"/>
+            <a:ext cx="136440" cy="119520"/>
           </a:xfrm>
           <a:prstGeom prst="ellipse">
             <a:avLst/>
@@ -7078,7 +7117,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3368160" y="5655240"/>
-            <a:ext cx="138600" cy="119880"/>
+            <a:ext cx="138240" cy="119520"/>
           </a:xfrm>
           <a:prstGeom prst="ellipse">
             <a:avLst/>
@@ -7117,9 +7156,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>549000</xdr:colOff>
+      <xdr:colOff>548640</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>127080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7133,7 +7172,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3475080" cy="898920"/>
+          <a:ext cx="3474720" cy="898560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7154,9 +7193,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>295200</xdr:colOff>
+      <xdr:colOff>294840</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>51840</xdr:rowOff>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7170,7 +7209,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="281160" y="2152440"/>
-          <a:ext cx="1477080" cy="385560"/>
+          <a:ext cx="1476720" cy="385200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7191,9 +7230,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>161640</xdr:colOff>
+      <xdr:colOff>161280</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7207,7 +7246,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3805200" y="2138400"/>
-          <a:ext cx="1477080" cy="390240"/>
+          <a:ext cx="1476720" cy="389880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7228,9 +7267,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>161640</xdr:colOff>
+      <xdr:colOff>161280</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7244,7 +7283,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3805200" y="3905280"/>
-          <a:ext cx="1477080" cy="385200"/>
+          <a:ext cx="1476720" cy="384840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7265,9 +7304,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>14040</xdr:colOff>
+      <xdr:colOff>13680</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>32760</xdr:rowOff>
+      <xdr:rowOff>32400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7281,7 +7320,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="731520" y="3914640"/>
-          <a:ext cx="1477080" cy="385200"/>
+          <a:ext cx="1476720" cy="384840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7307,9 +7346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1739880</xdr:colOff>
+      <xdr:colOff>1739520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>736920</xdr:rowOff>
+      <xdr:rowOff>736560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7323,7 +7362,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="1730520" cy="736920"/>
+          <a:ext cx="1730160" cy="736560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8054,7 +8093,7 @@
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G4" s="201" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="H4" s="202" t="n">
         <v>5600</v>
@@ -8062,7 +8101,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="201" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="H5" s="202" t="n">
         <v>600</v>
@@ -8070,7 +8109,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="201" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="H6" s="202" t="n">
         <v>7562.4</v>
@@ -8100,8 +8139,8 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M10" activeCellId="0" sqref="M10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8290,7 +8329,10 @@
       <c r="M7" s="11" t="n">
         <v>2326.72</v>
       </c>
-      <c r="N7" s="13"/>
+      <c r="N7" s="13" t="n">
+        <f aca="false">SUM(B7:M7)</f>
+        <v>26588.67</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="50" t="s">
@@ -8332,7 +8374,10 @@
       <c r="M8" s="11" t="n">
         <v>17589.42</v>
       </c>
-      <c r="N8" s="13"/>
+      <c r="N8" s="13" t="n">
+        <f aca="false">SUM(B8:M8)</f>
+        <v>224215.28</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="50" t="s">
@@ -8374,7 +8419,10 @@
       <c r="M9" s="11" t="n">
         <v>1200</v>
       </c>
-      <c r="N9" s="13"/>
+      <c r="N9" s="13" t="n">
+        <f aca="false">SUM(B9:M9)</f>
+        <v>22200</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="50" t="s">
@@ -8428,7 +8476,7 @@
         <f aca="false">SUM(M11:M24)</f>
         <v>2502.2</v>
       </c>
-      <c r="N10" s="56" t="n">
+      <c r="N10" s="13" t="n">
         <f aca="false">SUM(B10:M10)</f>
         <v>49517.64</v>
       </c>
@@ -8475,7 +8523,10 @@
       <c r="M11" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N11" s="13"/>
+      <c r="N11" s="13" t="n">
+        <f aca="false">SUM(B11:M11)</f>
+        <v>10857.8</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="50" t="s">
@@ -8517,7 +8568,10 @@
       <c r="M12" s="11" t="n">
         <v>42</v>
       </c>
-      <c r="N12" s="13"/>
+      <c r="N12" s="13" t="n">
+        <f aca="false">SUM(B12:M12)</f>
+        <v>532.33</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="50" t="s">
@@ -8559,7 +8613,10 @@
       <c r="M13" s="11" t="n">
         <v>1200</v>
       </c>
-      <c r="N13" s="13"/>
+      <c r="N13" s="13" t="n">
+        <f aca="false">SUM(B13:M13)</f>
+        <v>14400</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="50" t="s">
@@ -8601,7 +8658,10 @@
       <c r="M14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N14" s="13"/>
+      <c r="N14" s="13" t="n">
+        <f aca="false">SUM(B14:M14)</f>
+        <v>1156.86</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="50" t="s">
@@ -8643,7 +8703,10 @@
       <c r="M15" s="11" t="n">
         <v>83</v>
       </c>
-      <c r="N15" s="13"/>
+      <c r="N15" s="13" t="n">
+        <f aca="false">SUM(B15:M15)</f>
+        <v>998</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="50" t="s">
@@ -8685,7 +8748,10 @@
       <c r="M16" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N16" s="13"/>
+      <c r="N16" s="13" t="n">
+        <f aca="false">SUM(B16:M16)</f>
+        <v>447</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="50" t="s">
@@ -8727,7 +8793,10 @@
       <c r="M17" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N17" s="13"/>
+      <c r="N17" s="13" t="n">
+        <f aca="false">SUM(B17:M17)</f>
+        <v>2500</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="50" t="s">
@@ -8769,7 +8838,10 @@
       <c r="M18" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N18" s="25"/>
+      <c r="N18" s="13" t="n">
+        <f aca="false">SUM(B18:M18)</f>
+        <v>1376</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="50" t="s">
@@ -8811,7 +8883,10 @@
       <c r="M19" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N19" s="29"/>
+      <c r="N19" s="13" t="n">
+        <f aca="false">SUM(B19:M19)</f>
+        <v>2418.67</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="50" t="s">
@@ -8853,7 +8928,10 @@
       <c r="M20" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N20" s="29"/>
+      <c r="N20" s="13" t="n">
+        <f aca="false">SUM(B20:M20)</f>
+        <v>4865</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="50" t="s">
@@ -8895,7 +8973,10 @@
       <c r="M21" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N21" s="33"/>
+      <c r="N21" s="13" t="n">
+        <f aca="false">SUM(B21:M21)</f>
+        <v>3691.78</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="50" t="s">
@@ -8938,7 +9019,10 @@
       <c r="M22" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N22" s="33"/>
+      <c r="N22" s="13" t="n">
+        <f aca="false">SUM(B22:M22)</f>
+        <v>5097</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="50" t="s">
@@ -8980,7 +9064,10 @@
       <c r="M23" s="11" t="n">
         <v>677.2</v>
       </c>
-      <c r="N23" s="33"/>
+      <c r="N23" s="13" t="n">
+        <f aca="false">SUM(B23:M23)</f>
+        <v>677.2</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="50" t="s">
@@ -9022,7 +9109,10 @@
       <c r="M24" s="11" t="n">
         <v>500</v>
       </c>
-      <c r="N24" s="33"/>
+      <c r="N24" s="13" t="n">
+        <f aca="false">SUM(B24:M24)</f>
+        <v>500</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="50" t="s">
@@ -9064,7 +9154,10 @@
       <c r="M25" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N25" s="33"/>
+      <c r="N25" s="13" t="n">
+        <f aca="false">SUM(B25:M25)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="50" t="s">
@@ -9847,7 +9940,7 @@
         <v>56</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J4" s="70" t="n">
         <v>1</v>
@@ -9873,7 +9966,7 @@
       </c>
       <c r="H5" s="72"/>
       <c r="J5" s="73" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K5" s="73"/>
       <c r="L5" s="73"/>
@@ -9883,21 +9976,21 @@
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="75" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6" s="76" t="n">
         <f aca="false">META!C8</f>
         <v>0.184126430099499</v>
       </c>
       <c r="D6" s="77" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E6" s="78" t="n">
         <f aca="false">META!C14</f>
         <v>0.7854</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H6" s="76" t="n">
         <f aca="false">META!C20</f>
@@ -9921,7 +10014,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="38" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H8" s="79"/>
       <c r="J8" s="73"/>
@@ -9933,11 +10026,11 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D9" s="65" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E9" s="65"/>
       <c r="G9" s="79" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J9" s="73"/>
       <c r="K9" s="73"/>
@@ -9956,7 +10049,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="J11" s="82" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K11" s="82"/>
       <c r="L11" s="82"/>
@@ -10368,7 +10461,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10389,7 +10482,7 @@
     </row>
     <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="91" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C6" s="92"/>
       <c r="D6" s="93"/>
@@ -10412,7 +10505,7 @@
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="91" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C7" s="92"/>
       <c r="D7" s="95"/>
@@ -10435,14 +10528,14 @@
     </row>
     <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="91" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C8" s="92"/>
       <c r="D8" s="95"/>
       <c r="E8" s="95"/>
       <c r="F8" s="95"/>
       <c r="G8" s="97" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H8" s="98"/>
       <c r="I8" s="95"/>
@@ -10495,25 +10588,25 @@
       <c r="K10" s="67"/>
       <c r="L10" s="67"/>
       <c r="M10" s="103" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N10" s="103"/>
       <c r="O10" s="104" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P10" s="104" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="65" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
       <c r="D11" s="105"/>
       <c r="F11" s="106" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G11" s="107" t="n">
         <v>15000</v>
@@ -10524,33 +10617,33 @@
       <c r="K11" s="109"/>
       <c r="L11" s="109"/>
       <c r="M11" s="110" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N11" s="111" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O11" s="112" t="n">
         <v>0.06</v>
       </c>
       <c r="P11" s="111" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="113" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B12" s="114" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C12" s="114" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D12" s="115" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F12" s="106" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G12" s="116" t="n">
         <f aca="false">G11*12</f>
@@ -10562,10 +10655,10 @@
       <c r="K12" s="35"/>
       <c r="L12" s="35"/>
       <c r="M12" s="110" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N12" s="111" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O12" s="112" t="n">
         <v>0.112</v>
@@ -10576,7 +10669,7 @@
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="118" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B13" s="119" t="n">
         <f aca="false">F22</f>
@@ -10592,7 +10685,7 @@
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="106" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G13" s="107" t="n">
         <v>0</v>
@@ -10602,10 +10695,10 @@
       <c r="K13" s="35"/>
       <c r="L13" s="35"/>
       <c r="M13" s="110" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N13" s="111" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O13" s="112" t="n">
         <v>0.135</v>
@@ -10616,7 +10709,7 @@
     </row>
     <row r="14" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="118" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B14" s="119" t="n">
         <v>0.1633</v>
@@ -10630,7 +10723,7 @@
         <v>29394</v>
       </c>
       <c r="F14" s="106" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G14" s="122" t="n">
         <v>0.06</v>
@@ -10641,10 +10734,10 @@
       <c r="K14" s="35"/>
       <c r="L14" s="35"/>
       <c r="M14" s="110" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N14" s="111" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="O14" s="112" t="n">
         <v>0.16</v>
@@ -10655,7 +10748,7 @@
     </row>
     <row r="15" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="118" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B15" s="119" t="n">
         <v>0.3483</v>
@@ -10669,7 +10762,7 @@
         <v>62694</v>
       </c>
       <c r="F15" s="124" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G15" s="122" t="n">
         <f aca="false">F22</f>
@@ -10681,10 +10774,10 @@
       <c r="K15" s="35"/>
       <c r="L15" s="35"/>
       <c r="M15" s="110" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N15" s="111" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O15" s="112" t="n">
         <v>0.21</v>
@@ -10702,10 +10795,10 @@
       <c r="K16" s="35"/>
       <c r="L16" s="35"/>
       <c r="M16" s="110" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N16" s="111" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O16" s="112" t="n">
         <v>0.33</v>
@@ -10738,7 +10831,7 @@
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C20" s="130" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D20" s="130"/>
       <c r="E20" s="130"/>
@@ -10748,10 +10841,10 @@
       <c r="K20" s="35"/>
       <c r="L20" s="35"/>
       <c r="M20" s="103" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N20" s="103" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O20" s="103"/>
       <c r="P20" s="103"/>
@@ -10762,7 +10855,7 @@
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C21" s="131" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D21" s="131"/>
       <c r="E21" s="131"/>
@@ -10770,23 +10863,23 @@
       <c r="G21" s="127"/>
       <c r="M21" s="103"/>
       <c r="N21" s="103" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O21" s="103"/>
       <c r="P21" s="132" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="Q21" s="132" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="R21" s="132" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="S21" s="132" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="T21" s="132" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10795,7 +10888,7 @@
         <v>10800</v>
       </c>
       <c r="C22" s="134" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D22" s="135" t="n">
         <v>0</v>
@@ -10808,7 +10901,7 @@
       <c r="G22" s="136"/>
       <c r="I22" s="35"/>
       <c r="M22" s="110" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N22" s="137" t="n">
         <v>0.04</v>
@@ -10842,7 +10935,7 @@
       <c r="G23" s="136"/>
       <c r="I23" s="139"/>
       <c r="M23" s="110" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N23" s="137" t="n">
         <v>0.04</v>
@@ -10866,7 +10959,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M24" s="110" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N24" s="137" t="n">
         <v>0.04</v>
@@ -10890,7 +10983,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M25" s="110" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N25" s="137" t="n">
         <v>0.04</v>
@@ -10914,7 +11007,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M26" s="110" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N26" s="137" t="n">
         <v>0.04</v>
@@ -10933,12 +11026,12 @@
         <v>0.434</v>
       </c>
       <c r="T26" s="111" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M27" s="110" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N27" s="137" t="n">
         <v>0.35</v>
@@ -10957,12 +11050,12 @@
         <v>0.305</v>
       </c>
       <c r="T27" s="111" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="M28" s="140" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N28" s="140"/>
       <c r="O28" s="140"/>
@@ -10974,50 +11067,50 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="M29" s="141" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N29" s="142" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O29" s="143" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="P29" s="143"/>
       <c r="Q29" s="142" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="R29" s="142" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="S29" s="142" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="T29" s="142" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="57.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="M30" s="110" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N30" s="111" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="O30" s="140" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="P30" s="140"/>
       <c r="Q30" s="111" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="R30" s="111" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="S30" s="111" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="T30" s="111" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11083,7 +11176,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="35" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C3" s="35"/>
       <c r="D3" s="35"/>
@@ -11144,30 +11237,30 @@
       <c r="B5" s="148"/>
       <c r="C5" s="148"/>
       <c r="D5" s="149" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E5" s="149"/>
       <c r="F5" s="150" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G5" s="150"/>
       <c r="H5" s="150" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I5" s="150" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J5" s="150" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K5" s="150" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L5" s="150" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M5" s="151" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N5" s="93" t="n">
         <v>301.5</v>
@@ -11183,7 +11276,7 @@
     <row r="6" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="152"/>
       <c r="B6" s="153" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C6" s="153"/>
       <c r="D6" s="154" t="n">
@@ -11232,14 +11325,14 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="35" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C7" s="121" t="n">
         <v>30000</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="35" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F7" s="158" t="n">
         <f aca="false">F6*C7</f>
@@ -11322,25 +11415,25 @@
         <v>15354.33</v>
       </c>
       <c r="D12" s="165" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E12" s="165"/>
       <c r="F12" s="165"/>
       <c r="G12" s="165"/>
       <c r="H12" s="166" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I12" s="166" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L12" s="165" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M12" s="165" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N12" s="165"/>
       <c r="O12" s="165"/>
@@ -11351,10 +11444,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D13" s="110" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E13" s="140" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F13" s="140"/>
       <c r="G13" s="140"/>
@@ -11366,23 +11459,23 @@
       </c>
       <c r="L13" s="165"/>
       <c r="M13" s="165" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N13" s="165"/>
       <c r="O13" s="167" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="P13" s="167" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q13" s="167" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R13" s="167" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S13" s="167" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11391,10 +11484,10 @@
         <v>750</v>
       </c>
       <c r="D14" s="110" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E14" s="140" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F14" s="140"/>
       <c r="G14" s="140"/>
@@ -11405,7 +11498,7 @@
         <v>9360</v>
       </c>
       <c r="L14" s="110" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M14" s="137" t="n">
         <v>0.04</v>
@@ -11433,10 +11526,10 @@
         <v>12.5</v>
       </c>
       <c r="D15" s="110" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E15" s="140" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F15" s="140"/>
       <c r="G15" s="140"/>
@@ -11447,7 +11540,7 @@
         <v>17640</v>
       </c>
       <c r="L15" s="110" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M15" s="137" t="n">
         <v>0.04</v>
@@ -11471,10 +11564,10 @@
     </row>
     <row r="16" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D16" s="110" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E16" s="140" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F16" s="140"/>
       <c r="G16" s="140"/>
@@ -11485,7 +11578,7 @@
         <v>35640</v>
       </c>
       <c r="L16" s="110" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M16" s="137" t="n">
         <v>0.04</v>
@@ -11509,10 +11602,10 @@
     </row>
     <row r="17" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D17" s="110" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E17" s="140" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F17" s="140"/>
       <c r="G17" s="140"/>
@@ -11523,7 +11616,7 @@
         <v>125640</v>
       </c>
       <c r="L17" s="110" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M17" s="137" t="n">
         <v>0.04</v>
@@ -11547,10 +11640,10 @@
     </row>
     <row r="18" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D18" s="110" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E18" s="140" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F18" s="140"/>
       <c r="G18" s="140"/>
@@ -11561,7 +11654,7 @@
         <v>648000</v>
       </c>
       <c r="L18" s="110" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M18" s="137" t="n">
         <v>0.04</v>
@@ -11580,12 +11673,12 @@
         <v>0.434</v>
       </c>
       <c r="S18" s="111" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L19" s="110" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M19" s="137" t="n">
         <v>0.35</v>
@@ -11604,12 +11697,12 @@
         <v>0.305</v>
       </c>
       <c r="S19" s="111" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="L20" s="140" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M20" s="140"/>
       <c r="N20" s="140"/>
@@ -11621,26 +11714,26 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="L21" s="141" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M21" s="142" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N21" s="143" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O21" s="143"/>
       <c r="P21" s="142" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q21" s="142" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R21" s="142" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S21" s="142" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="57.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11649,26 +11742,26 @@
         <v>631.6</v>
       </c>
       <c r="L22" s="110" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="M22" s="111" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N22" s="140" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O22" s="140"/>
       <c r="P22" s="111" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q22" s="111" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="R22" s="111" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="S22" s="111" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -11734,15 +11827,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="41" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="168" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C2" s="169" t="n">
         <v>36254</v>
@@ -11757,7 +11850,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="41" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C3" s="172" t="n">
         <v>105</v>
@@ -11773,7 +11866,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="41" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C4" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!L26</f>
@@ -11792,15 +11885,15 @@
         <v>23017.16</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I4" s="172" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C5" s="179" t="n">
         <f aca="false">'LIVRO CAIXA'!L6-'LIVRO CAIXA'!K6</f>
@@ -11823,7 +11916,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="41" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C6" s="178" t="n">
         <f aca="false">META!M7-META!M6</f>
@@ -11840,7 +11933,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="41" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F8" s="182"/>
     </row>
@@ -11852,15 +11945,15 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="41" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C11" s="41" t="n">
         <v>45000</v>
@@ -11871,7 +11964,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C12" s="41" t="n">
         <v>43000</v>
@@ -11882,7 +11975,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C13" s="41" t="n">
         <v>54000</v>
@@ -11893,7 +11986,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="41" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C14" s="41" t="n">
         <v>60000</v>
@@ -11904,7 +11997,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="41" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C15" s="41" t="n">
         <v>30000</v>
@@ -11915,7 +12008,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="41" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C16" s="41" t="n">
         <v>80000</v>
@@ -11926,7 +12019,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="41" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C17" s="41" t="n">
         <v>35000</v>
@@ -11937,7 +12030,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C18" s="41" t="n">
         <v>15000</v>
@@ -11948,7 +12041,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="41" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C19" s="41" t="n">
         <v>12000</v>
@@ -11959,7 +12052,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="41" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C20" s="41" t="n">
         <v>45000</v>
@@ -11970,7 +12063,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="41" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C21" s="41" t="n">
         <v>80000</v>
@@ -11981,7 +12074,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="41" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C22" s="41" t="n">
         <v>81000</v>
@@ -11992,25 +12085,25 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="41" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="41" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="41" t="str">
         <f aca="false">'LIVRO CAIXA'!A11</f>
-        <v>DESPESA COM ANESTESIA</v>
+        <v>DESPESACOMANESTESIA</v>
       </c>
       <c r="C27" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!B11</f>
         <v>1330.5</v>
       </c>
       <c r="G27" s="50" t="s">
-        <v>30</v>
+        <v>151</v>
       </c>
       <c r="H27" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L11</f>
@@ -12020,14 +12113,14 @@
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="41" t="str">
         <f aca="false">'LIVRO CAIXA'!A18</f>
-        <v>DESPESA COM ALIMENTAÇÃO</v>
+        <v>DESPESACOMALIMENTACAO</v>
       </c>
       <c r="C28" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!B18</f>
         <v>408</v>
       </c>
       <c r="G28" s="50" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="H28" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L12</f>
@@ -12037,14 +12130,14 @@
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="41" t="str">
         <f aca="false">'LIVRO CAIXA'!A19</f>
-        <v>DESPESA COM COMBUSTÍVEL</v>
+        <v>DESPESACOMCOMBUSTIVEL</v>
       </c>
       <c r="C29" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!B19</f>
         <v>500</v>
       </c>
       <c r="G29" s="50" t="s">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="H29" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L13</f>
@@ -12054,14 +12147,14 @@
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="41" t="str">
         <f aca="false">'LIVRO CAIXA'!A21</f>
-        <v>DESPESA COM PLANO DE SAÚDE</v>
+        <v>DESPESACOMPLANODESAUDE</v>
       </c>
       <c r="C30" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!B21</f>
         <v>430</v>
       </c>
       <c r="G30" s="50" t="s">
-        <v>33</v>
+        <v>154</v>
       </c>
       <c r="H30" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L14</f>
@@ -12071,14 +12164,14 @@
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="41" t="str">
         <f aca="false">'LIVRO CAIXA'!A22</f>
-        <v>DESPESA COM LAZER</v>
+        <v>DESPESACOMLAZER</v>
       </c>
       <c r="C31" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!B22</f>
         <v>230</v>
       </c>
       <c r="G31" s="50" t="s">
-        <v>34</v>
+        <v>155</v>
       </c>
       <c r="H31" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L15</f>
@@ -12095,7 +12188,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="50" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="H32" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L16</f>
@@ -12112,7 +12205,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="50" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="H33" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L17</f>
@@ -12129,7 +12222,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="50" t="s">
-        <v>37</v>
+        <v>158</v>
       </c>
       <c r="H34" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L18</f>
@@ -12139,7 +12232,7 @@
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="175"/>
       <c r="G35" s="50" t="s">
-        <v>38</v>
+        <v>159</v>
       </c>
       <c r="H35" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L19</f>
@@ -12149,7 +12242,7 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="175"/>
       <c r="G36" s="50" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
       <c r="H36" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L20</f>
@@ -12158,7 +12251,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G37" s="50" t="s">
-        <v>40</v>
+        <v>161</v>
       </c>
       <c r="H37" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L21</f>
@@ -12167,10 +12260,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="41" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="G38" s="50" t="s">
-        <v>41</v>
+        <v>163</v>
       </c>
       <c r="H38" s="41" t="n">
         <f aca="false">'LIVRO CAIXA'!L22</f>
@@ -12188,10 +12281,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="41" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="D40" s="41" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="G40" s="50" t="s">
         <v>43</v>
@@ -12203,7 +12296,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="41" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="C41" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!B6</f>
@@ -12222,7 +12315,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="41" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="C42" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!C6</f>
@@ -12235,7 +12328,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="41" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="C43" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!D6</f>
@@ -12248,7 +12341,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="41" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="C44" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!E6</f>
@@ -12261,7 +12354,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="41" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="C45" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!F6</f>
@@ -12274,7 +12367,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="41" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="C46" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!G6</f>
@@ -12287,7 +12380,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="41" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="C47" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!H6</f>
@@ -12300,7 +12393,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="41" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="C48" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!I6</f>
@@ -12313,7 +12406,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="41" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="C49" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!J6</f>
@@ -12326,7 +12419,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="41" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="C50" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!K6</f>
@@ -12339,7 +12432,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="41" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="C51" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!L6</f>
@@ -12352,7 +12445,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="41" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="C52" s="175" t="n">
         <f aca="false">'LIVRO CAIXA'!M6</f>
@@ -12372,7 +12465,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="41" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -12430,38 +12523,38 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="186" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="C2" s="186"/>
       <c r="D2" s="186"/>
       <c r="F2" s="186" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="G2" s="186"/>
       <c r="H2" s="186"/>
       <c r="J2" s="186" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="K2" s="186"/>
       <c r="L2" s="186"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="187" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="C3" s="187"/>
       <c r="D3" s="188" t="n">
         <v>270000</v>
       </c>
       <c r="F3" s="187" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="G3" s="187"/>
       <c r="H3" s="188" t="n">
         <v>270000</v>
       </c>
       <c r="J3" s="187" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="K3" s="187"/>
       <c r="L3" s="188" t="n">
@@ -12470,12 +12563,12 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="189" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="C4" s="189"/>
       <c r="D4" s="189"/>
       <c r="F4" s="189" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G4" s="190" t="n">
         <v>0.05</v>
@@ -12485,7 +12578,7 @@
         <v>13500</v>
       </c>
       <c r="J4" s="189" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="K4" s="190" t="n">
         <v>0.05</v>
@@ -12497,7 +12590,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="187" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="C5" s="187"/>
       <c r="D5" s="188" t="n">
@@ -12505,7 +12598,7 @@
         <v>270000</v>
       </c>
       <c r="F5" s="189" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="G5" s="190" t="n">
         <v>0.0065</v>
@@ -12515,7 +12608,7 @@
         <v>1755</v>
       </c>
       <c r="J5" s="189" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="K5" s="190" t="n">
         <v>0.06</v>
@@ -12527,14 +12620,14 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="189" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="C6" s="189"/>
       <c r="D6" s="192" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="189" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G6" s="190" t="n">
         <v>0.03</v>
@@ -12544,7 +12637,7 @@
         <v>8100</v>
       </c>
       <c r="J6" s="189" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K6" s="190" t="n">
         <v>0.02</v>
@@ -12556,14 +12649,14 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="189" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="C7" s="189"/>
       <c r="D7" s="192" t="n">
         <v>0</v>
       </c>
       <c r="F7" s="189" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="G7" s="190" t="n">
         <v>0.05</v>
@@ -12572,7 +12665,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="189" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="K7" s="190" t="n">
         <v>0.12</v>
@@ -12584,7 +12677,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="187" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="C8" s="187"/>
       <c r="D8" s="188" t="n">
@@ -12592,7 +12685,7 @@
         <v>270000</v>
       </c>
       <c r="F8" s="187" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="G8" s="187"/>
       <c r="H8" s="188" t="n">
@@ -12600,7 +12693,7 @@
         <v>246645</v>
       </c>
       <c r="J8" s="189" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="K8" s="190" t="n">
         <v>0.017</v>
@@ -12612,7 +12705,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="189" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="C9" s="190" t="n">
         <v>0.0765</v>
@@ -12622,14 +12715,14 @@
         <v>20655</v>
       </c>
       <c r="F9" s="189" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="G9" s="189"/>
       <c r="H9" s="192" t="n">
         <v>0</v>
       </c>
       <c r="J9" s="189" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="K9" s="190" t="n">
         <v>0.07</v>
@@ -12641,7 +12734,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="187" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="G10" s="187"/>
       <c r="H10" s="188" t="n">
@@ -12649,7 +12742,7 @@
         <v>246645</v>
       </c>
       <c r="J10" s="187" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="K10" s="187"/>
       <c r="L10" s="188" t="n">
@@ -12664,14 +12757,14 @@
         <v>1721.25</v>
       </c>
       <c r="F11" s="189" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="G11" s="189"/>
       <c r="H11" s="192" t="n">
         <v>0</v>
       </c>
       <c r="J11" s="189" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="K11" s="189"/>
       <c r="L11" s="192" t="n">
@@ -12681,14 +12774,14 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F12" s="189" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="G12" s="189"/>
       <c r="H12" s="192" t="n">
         <v>0</v>
       </c>
       <c r="J12" s="187" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="K12" s="187"/>
       <c r="L12" s="188" t="n">
@@ -12699,14 +12792,14 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F13" s="189" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="G13" s="189"/>
       <c r="H13" s="192" t="n">
         <v>0</v>
       </c>
       <c r="J13" s="189" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="K13" s="189"/>
       <c r="L13" s="192" t="n">
@@ -12716,7 +12809,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F14" s="187" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="G14" s="187"/>
       <c r="H14" s="188" t="n">
@@ -12724,7 +12817,7 @@
         <v>246645</v>
       </c>
       <c r="J14" s="189" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="K14" s="189"/>
       <c r="L14" s="192" t="n">
@@ -12735,7 +12828,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="189" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="G15" s="190" t="n">
         <v>0.09</v>
@@ -12745,7 +12838,7 @@
         <v>2916</v>
       </c>
       <c r="J15" s="189" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="K15" s="189"/>
       <c r="L15" s="192" t="n">
@@ -12755,7 +12848,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="189" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="G16" s="190" t="n">
         <v>0.15</v>
@@ -12765,7 +12858,7 @@
         <v>3240</v>
       </c>
       <c r="J16" s="187" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="K16" s="187"/>
       <c r="L16" s="188" t="n">
@@ -12775,7 +12868,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="196" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="G17" s="190" t="n">
         <v>0.1</v>
@@ -12785,7 +12878,7 @@
         <v>2640</v>
       </c>
       <c r="J17" s="189" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="K17" s="190" t="n">
         <v>0.07</v>
@@ -12797,7 +12890,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J18" s="189" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="K18" s="190" t="n">
         <v>0.07</v>
@@ -12812,7 +12905,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="199" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="C20" s="199"/>
       <c r="D20" s="200" t="n">
@@ -12820,7 +12913,7 @@
         <v>249345</v>
       </c>
       <c r="F20" s="199" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="G20" s="199"/>
       <c r="H20" s="200" t="n">
@@ -12828,7 +12921,7 @@
         <v>237849</v>
       </c>
       <c r="J20" s="199" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="K20" s="199"/>
       <c r="L20" s="200" t="n">
@@ -12838,7 +12931,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="184" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="G21" s="198"/>
       <c r="H21" s="197" t="n">

</xml_diff>

<commit_message>
change: atualiza dados financeiros e corrige formatação no fluxo
</commit_message>
<xml_diff>
--- a/app/fluxo.xlsx
+++ b/app/fluxo.xlsx
@@ -713,17 +713,17 @@
     <numFmt numFmtId="165" formatCode="&quot;R$ &quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="[$R$-416]\ #,##0.00;[RED]\-[$R$-416]\ #,##0.00"/>
-    <numFmt numFmtId="168" formatCode="General"/>
-    <numFmt numFmtId="169" formatCode="_-&quot;R$ &quot;* #,##0.00_-;&quot;-R$ &quot;* #,##0.00_-;_-&quot;R$ &quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="[&gt;=1000]#,##0,\K;0"/>
-    <numFmt numFmtId="171" formatCode="#,##0"/>
-    <numFmt numFmtId="172" formatCode="_-&quot;R$&quot;* #,##0.00_-;&quot;-R$&quot;* #,##0.00_-;_-&quot;R$&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="0.00%"/>
-    <numFmt numFmtId="174" formatCode="#,##0.00"/>
-    <numFmt numFmtId="175" formatCode="&quot;R$&quot;#,##0.00"/>
-    <numFmt numFmtId="176" formatCode="0.000000000000000%"/>
-    <numFmt numFmtId="177" formatCode="0.000000%"/>
-    <numFmt numFmtId="178" formatCode="&quot;R$ &quot;#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;R$ &quot;* #,##0.00_-;&quot;-R$ &quot;* #,##0.00_-;_-&quot;R$ &quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="[&gt;=1000]#,##0,\K;0"/>
+    <numFmt numFmtId="170" formatCode="#,##0"/>
+    <numFmt numFmtId="171" formatCode="_-&quot;R$&quot;* #,##0.00_-;&quot;-R$&quot;* #,##0.00_-;_-&quot;R$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="0.00%"/>
+    <numFmt numFmtId="173" formatCode="#,##0.00"/>
+    <numFmt numFmtId="174" formatCode="&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="175" formatCode="0.000000000000000%"/>
+    <numFmt numFmtId="176" formatCode="0.000000%"/>
+    <numFmt numFmtId="177" formatCode="&quot;R$ &quot;#,##0.000"/>
+    <numFmt numFmtId="178" formatCode="General"/>
     <numFmt numFmtId="179" formatCode="_-&quot;R$ &quot;* #,##0_-;&quot;-R$ &quot;* #,##0_-;_-&quot;R$ &quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="[$R$ -416]#,##0"/>
   </numFmts>
@@ -1598,7 +1598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
@@ -1835,7 +1835,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1863,7 +1863,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="7" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1939,7 +1939,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="14" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="10" fillId="14" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1995,7 +1995,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2043,7 +2043,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="34" fillId="2" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="34" fillId="2" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2059,35 +2059,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="172" fontId="26" fillId="17" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="17" borderId="24" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="173" fontId="26" fillId="17" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="33" fillId="17" borderId="24" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="26" fillId="17" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2099,11 +2099,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="36" fillId="17" borderId="25" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="36" fillId="17" borderId="25" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="36" fillId="2" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="36" fillId="2" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2127,7 +2127,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="33" fillId="2" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="33" fillId="2" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2143,11 +2143,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="41" fillId="2" borderId="27" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="41" fillId="2" borderId="27" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="42" fillId="2" borderId="27" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="42" fillId="2" borderId="27" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2155,19 +2155,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="26" fillId="17" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="26" fillId="17" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="41" fillId="2" borderId="28" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="174" fontId="41" fillId="2" borderId="28" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="44" fillId="2" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="44" fillId="2" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2199,7 +2199,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2231,15 +2231,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="2" borderId="36" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="175" fontId="4" fillId="2" borderId="36" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2255,19 +2255,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2287,19 +2287,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="47" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="178" fontId="47" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2307,7 +2307,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="47" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="178" fontId="47" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2319,7 +2319,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="47" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="47" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2335,7 +2335,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2371,7 +2371,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="26" fillId="20" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="26" fillId="20" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2419,7 +2419,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2684,7 +2684,7 @@
                 <c:formatCode>"R$ "#,##0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>19268.14</c:v>
+                  <c:v>6417.14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2858,11 +2858,11 @@
         </c:ser>
         <c:gapWidth val="65"/>
         <c:overlap val="0"/>
-        <c:axId val="1415943"/>
-        <c:axId val="38346707"/>
+        <c:axId val="41382608"/>
+        <c:axId val="3275739"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1415943"/>
+        <c:axId val="41382608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,7 +2894,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38346707"/>
+        <c:crossAx val="3275739"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2902,7 +2902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38346707"/>
+        <c:axId val="3275739"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2944,7 +2944,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1415943"/>
+        <c:crossAx val="41382608"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -3118,7 +3118,7 @@
                 <c:formatCode>"R$ "#,##0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>14278.85</c:v>
+                  <c:v>1427.85</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2400</c:v>
@@ -4004,10 +4004,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.136058109280139"/>
-          <c:y val="0.0409829237817576"/>
-          <c:w val="0.727883781439722"/>
-          <c:h val="0.641149521032903"/>
+          <c:x val="0.136065484902694"/>
+          <c:y val="0.0409863378873709"/>
+          <c:w val="0.727869030194612"/>
+          <c:h val="0.64111962679107"/>
         </c:manualLayout>
       </c:layout>
       <c:doughnutChart>
@@ -4847,44 +4847,44 @@
                 <c:formatCode>_-"R$ "* #,##0_-;"-R$ "* #,##0_-;_-"R$ "* \-??_-;_-@_-</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>20491</c:v>
+                  <c:v>6099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21280.56</c:v>
+                  <c:v>7368.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24778.27</c:v>
+                  <c:v>6176.27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18951.26</c:v>
+                  <c:v>4837.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23712.83</c:v>
+                  <c:v>6220.83</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20092.32</c:v>
+                  <c:v>4302.32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24959.52</c:v>
+                  <c:v>5394.52</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29352.73</c:v>
+                  <c:v>8741.73</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25984.02</c:v>
+                  <c:v>8065.02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23017.16</c:v>
+                  <c:v>5602.16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19268.14</c:v>
+                  <c:v>6417.14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="11260215"/>
-        <c:axId val="85526313"/>
+        <c:axId val="7963565"/>
+        <c:axId val="64460007"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4997,40 +4997,40 @@
                 <c:formatCode>_-"R$ "* #,##0_-;"-R$ "* #,##0_-;_-"R$ "* \-??_-;_-@_-</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>20491</c:v>
+                  <c:v>6099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21280.56</c:v>
+                  <c:v>7368.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24778.27</c:v>
+                  <c:v>6176.27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18951.26</c:v>
+                  <c:v>4837.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23712.83</c:v>
+                  <c:v>6220.83</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20092.32</c:v>
+                  <c:v>4302.32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24959.52</c:v>
+                  <c:v>5394.52</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29352.73</c:v>
+                  <c:v>8741.73</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25984.02</c:v>
+                  <c:v>8065.02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23017.16</c:v>
+                  <c:v>5602.16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19268.14</c:v>
+                  <c:v>6417.14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21116.14</c:v>
+                  <c:v>5285.14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5045,11 +5045,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="11260215"/>
-        <c:axId val="85526313"/>
+        <c:axId val="7963565"/>
+        <c:axId val="64460007"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="11260215"/>
+        <c:axId val="7963565"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5081,7 +5081,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85526313"/>
+        <c:crossAx val="64460007"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5089,7 +5089,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85526313"/>
+        <c:axId val="64460007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5128,7 +5128,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11260215"/>
+        <c:crossAx val="7963565"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5162,9 +5162,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1129680</xdr:colOff>
+      <xdr:colOff>1129320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>736200</xdr:rowOff>
+      <xdr:rowOff>735840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5178,7 +5178,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="1851840" cy="736200"/>
+          <a:ext cx="1851480" cy="735840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5204,9 +5204,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>157680</xdr:colOff>
+      <xdr:colOff>157320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5220,7 +5220,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3552480" cy="898200"/>
+          <a:ext cx="3552120" cy="897840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5246,9 +5246,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1129680</xdr:colOff>
+      <xdr:colOff>1129320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>736200</xdr:rowOff>
+      <xdr:rowOff>735840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5262,7 +5262,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="1851840" cy="736200"/>
+          <a:ext cx="1851480" cy="735840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5288,9 +5288,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>303480</xdr:colOff>
+      <xdr:colOff>303120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5299,7 +5299,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="2862360"/>
-        <a:ext cx="4018320" cy="2298600"/>
+        <a:ext cx="4017960" cy="2298240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5318,9 +5318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>491400</xdr:colOff>
+      <xdr:colOff>491040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5329,7 +5329,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3030840" y="2736000"/>
-        <a:ext cx="3883680" cy="2837880"/>
+        <a:ext cx="3883320" cy="2837520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5348,9 +5348,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1391400</xdr:colOff>
+      <xdr:colOff>1391040</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5359,7 +5359,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2995200" y="2670120"/>
-        <a:ext cx="10031400" cy="2926800"/>
+        <a:ext cx="10031040" cy="2926440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5378,9 +5378,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
+      <xdr:colOff>497880</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5394,7 +5394,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3481560" cy="895680"/>
+          <a:ext cx="3481200" cy="895320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5420,9 +5420,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>188640</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5432,7 +5432,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7120080" y="1041120"/>
-          <a:ext cx="6967800" cy="4291200"/>
+          <a:ext cx="6967440" cy="4290840"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5472,9 +5472,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>331920</xdr:colOff>
+      <xdr:colOff>331560</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5483,7 +5483,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7589880" y="982440"/>
-        <a:ext cx="6640920" cy="4321440"/>
+        <a:ext cx="6640560" cy="4321080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5502,9 +5502,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>456120</xdr:colOff>
+      <xdr:colOff>455760</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5514,7 +5514,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="520560" y="1136520"/>
-          <a:ext cx="2861640" cy="1512360"/>
+          <a:ext cx="2861280" cy="1512000"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5554,9 +5554,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>576000</xdr:colOff>
+      <xdr:colOff>575640</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>46080</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5566,7 +5566,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533160" y="1215360"/>
-          <a:ext cx="774360" cy="364320"/>
+          <a:ext cx="774000" cy="363960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5620,9 +5620,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>107640</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5632,7 +5632,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="520560" y="1702800"/>
-          <a:ext cx="1782000" cy="471960"/>
+          <a:ext cx="1781640" cy="471600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5687,9 +5687,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>370080</xdr:colOff>
+      <xdr:colOff>369720</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5699,7 +5699,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2628000" y="1228680"/>
-          <a:ext cx="668160" cy="525240"/>
+          <a:ext cx="667800" cy="524880"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5739,9 +5739,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>313200</xdr:colOff>
+      <xdr:colOff>312840</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:rowOff>173520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5761,7 +5761,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2677320" y="1307520"/>
-          <a:ext cx="561960" cy="399960"/>
+          <a:ext cx="561600" cy="399600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5782,9 +5782,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>132120</xdr:colOff>
+      <xdr:colOff>131760</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -5794,9 +5794,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="3838680" y="1140840"/>
-          <a:ext cx="2877120" cy="1512360"/>
+          <a:ext cx="2876760" cy="1512000"/>
           <a:chOff x="3838680" y="1140840"/>
-          <a:chExt cx="2877120" cy="1512360"/>
+          <a:chExt cx="2876760" cy="1512000"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -5807,7 +5807,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3857400" y="1140840"/>
-            <a:ext cx="2858400" cy="1512360"/>
+            <a:ext cx="2858040" cy="1512000"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst>
@@ -5844,7 +5844,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3944880" y="1226520"/>
-            <a:ext cx="1308600" cy="331920"/>
+            <a:ext cx="1308240" cy="331560"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -5895,7 +5895,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="5931720" y="1217160"/>
-            <a:ext cx="658440" cy="525240"/>
+            <a:ext cx="658080" cy="524880"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst>
@@ -5942,7 +5942,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="6005880" y="1264680"/>
-            <a:ext cx="506880" cy="408240"/>
+            <a:ext cx="506520" cy="407880"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -5960,7 +5960,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3838680" y="1655280"/>
-            <a:ext cx="1415520" cy="341280"/>
+            <a:ext cx="1415160" cy="340920"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6012,7 +6012,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="5352480" y="2347560"/>
-            <a:ext cx="1203480" cy="216000"/>
+            <a:ext cx="1203120" cy="215640"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6067,9 +6067,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>486360</xdr:colOff>
+      <xdr:colOff>486000</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6079,7 +6079,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="550800" y="2964600"/>
-          <a:ext cx="2861640" cy="1512360"/>
+          <a:ext cx="2861280" cy="1512000"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6119,9 +6119,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>134640</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6131,7 +6131,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3857040" y="2958840"/>
-          <a:ext cx="2861640" cy="1512360"/>
+          <a:ext cx="2861280" cy="1512000"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6171,9 +6171,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>30600</xdr:colOff>
+      <xdr:colOff>30240</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>55080</xdr:rowOff>
+      <xdr:rowOff>54720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6183,7 +6183,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5945760" y="3035160"/>
-          <a:ext cx="668520" cy="525240"/>
+          <a:ext cx="668160" cy="524880"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6223,9 +6223,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>513000</xdr:colOff>
+      <xdr:colOff>512640</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6239,7 +6239,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6071400" y="3095640"/>
-          <a:ext cx="293760" cy="392040"/>
+          <a:ext cx="293400" cy="391680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6260,9 +6260,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>84600</xdr:colOff>
+      <xdr:colOff>84240</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
+      <xdr:rowOff>158040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6272,7 +6272,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3981600" y="3019320"/>
-          <a:ext cx="1223640" cy="263160"/>
+          <a:ext cx="1223280" cy="262800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6326,9 +6326,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>335520</xdr:colOff>
+      <xdr:colOff>335160</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>71280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6338,7 +6338,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4064040" y="3426120"/>
-          <a:ext cx="1392120" cy="341280"/>
+          <a:ext cx="1391760" cy="340920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6393,9 +6393,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>47160</xdr:colOff>
+      <xdr:colOff>46800</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6405,7 +6405,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5263560" y="4057560"/>
-          <a:ext cx="1367280" cy="292320"/>
+          <a:ext cx="1366920" cy="291960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6459,9 +6459,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>13320</xdr:colOff>
+      <xdr:colOff>12960</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6471,7 +6471,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2005920" y="2304720"/>
-          <a:ext cx="1665000" cy="299520"/>
+          <a:ext cx="1664640" cy="299160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6525,9 +6525,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>124560</xdr:colOff>
+      <xdr:colOff>124200</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6537,7 +6537,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="585000" y="3047400"/>
-          <a:ext cx="1734120" cy="364320"/>
+          <a:ext cx="1733760" cy="363960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6591,9 +6591,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>370080</xdr:colOff>
+      <xdr:colOff>369720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>93240</xdr:rowOff>
+      <xdr:rowOff>92880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6603,7 +6603,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2628000" y="3073320"/>
-          <a:ext cx="668160" cy="525240"/>
+          <a:ext cx="667800" cy="524880"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6643,9 +6643,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>316800</xdr:colOff>
+      <xdr:colOff>316440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6659,7 +6659,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2729160" y="3094560"/>
-          <a:ext cx="513720" cy="414000"/>
+          <a:ext cx="513360" cy="413640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6680,9 +6680,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>184320</xdr:colOff>
+      <xdr:colOff>183960</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>88560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6692,7 +6692,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="596880" y="3503160"/>
-          <a:ext cx="1782000" cy="471960"/>
+          <a:ext cx="1781640" cy="471600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6747,9 +6747,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>70560</xdr:colOff>
+      <xdr:colOff>70200</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6759,7 +6759,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2063160" y="4114800"/>
-          <a:ext cx="1665000" cy="299160"/>
+          <a:ext cx="1664640" cy="298800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6813,9 +6813,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>427320</xdr:colOff>
+      <xdr:colOff>426960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -6825,9 +6825,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="210240" y="4848120"/>
-          <a:ext cx="11189880" cy="3760920"/>
+          <a:ext cx="11189520" cy="3760560"/>
           <a:chOff x="210240" y="4848120"/>
-          <a:chExt cx="11189880" cy="3760920"/>
+          <a:chExt cx="11189520" cy="3760560"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -6838,7 +6838,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="1405080" y="4848120"/>
-            <a:ext cx="2574000" cy="417600"/>
+            <a:ext cx="2573640" cy="417240"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6887,7 +6887,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3393000" y="5334120"/>
-            <a:ext cx="1794240" cy="343080"/>
+            <a:ext cx="1793880" cy="342720"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6938,7 +6938,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="1369800" y="5315040"/>
-            <a:ext cx="1794240" cy="343080"/>
+            <a:ext cx="1793880" cy="342720"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6989,7 +6989,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="1446480" y="5541480"/>
-            <a:ext cx="1949400" cy="541440"/>
+            <a:ext cx="1949040" cy="541080"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -7041,7 +7041,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3573000" y="5579640"/>
-            <a:ext cx="1949400" cy="541440"/>
+            <a:ext cx="1949040" cy="541080"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -7092,7 +7092,7 @@
         </xdr:nvGraphicFramePr>
         <xdr:xfrm>
           <a:off x="210240" y="6302160"/>
-          <a:ext cx="11189880" cy="2306880"/>
+          <a:ext cx="11189520" cy="2306520"/>
         </xdr:xfrm>
         <a:graphic>
           <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7108,7 +7108,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="1388880" y="5659200"/>
-            <a:ext cx="136080" cy="119160"/>
+            <a:ext cx="135720" cy="118800"/>
           </a:xfrm>
           <a:prstGeom prst="ellipse">
             <a:avLst/>
@@ -7143,7 +7143,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3368160" y="5655240"/>
-            <a:ext cx="137880" cy="119160"/>
+            <a:ext cx="137520" cy="118800"/>
           </a:xfrm>
           <a:prstGeom prst="ellipse">
             <a:avLst/>
@@ -7182,9 +7182,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>548280</xdr:colOff>
+      <xdr:colOff>547920</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7198,7 +7198,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3474360" cy="898200"/>
+          <a:ext cx="3474000" cy="897840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7219,9 +7219,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>294480</xdr:colOff>
+      <xdr:colOff>294120</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>51120</xdr:rowOff>
+      <xdr:rowOff>50760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7235,7 +7235,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="281160" y="2152440"/>
-          <a:ext cx="1476360" cy="384840"/>
+          <a:ext cx="1476000" cy="384480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7256,9 +7256,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>160920</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7272,7 +7272,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3805200" y="2138400"/>
-          <a:ext cx="1476360" cy="389520"/>
+          <a:ext cx="1476000" cy="389160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7293,9 +7293,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>160920</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7309,7 +7309,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3805200" y="3905280"/>
-          <a:ext cx="1476360" cy="384480"/>
+          <a:ext cx="1476000" cy="384120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7330,9 +7330,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>13320</xdr:colOff>
+      <xdr:colOff>12960</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7346,7 +7346,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="731520" y="3914640"/>
-          <a:ext cx="1476360" cy="384480"/>
+          <a:ext cx="1476000" cy="384120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7372,9 +7372,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1739160</xdr:colOff>
+      <xdr:colOff>1738800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>736200</xdr:rowOff>
+      <xdr:rowOff>735840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7388,7 +7388,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="1729800" cy="736200"/>
+          <a:ext cx="1729440" cy="735840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7699,58 +7699,58 @@
       </c>
       <c r="C7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!B6</f>
-        <v>20491</v>
+        <v>6099</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!D6</f>
-        <v>24778.27</v>
+        <v>6176.27</v>
       </c>
       <c r="F7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!E6</f>
-        <v>18951.26</v>
+        <v>4837.26</v>
       </c>
       <c r="G7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!F6</f>
-        <v>23712.83</v>
+        <v>6220.83</v>
       </c>
       <c r="H7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!G6</f>
-        <v>20092.32</v>
+        <v>4302.32</v>
       </c>
       <c r="I7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!H6</f>
-        <v>24959.52</v>
+        <v>5394.52</v>
       </c>
       <c r="J7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!I6</f>
-        <v>29352.73</v>
+        <v>8741.73</v>
       </c>
       <c r="K7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!J6</f>
-        <v>25984.02</v>
+        <v>8065.02</v>
       </c>
       <c r="L7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!K6</f>
-        <v>23017.16</v>
+        <v>5602.16</v>
       </c>
       <c r="M7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!L6</f>
-        <v>19268.14</v>
+        <v>6417.14</v>
       </c>
       <c r="N7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!M6</f>
-        <v>21116.14</v>
+        <v>5285.14</v>
       </c>
       <c r="O7" s="16" t="n">
         <f aca="false">SUM(C7:N7)</f>
-        <v>251723.39</v>
+        <v>67141.39</v>
       </c>
       <c r="Q7" s="17" t="n">
         <f aca="false">D7-C7</f>
-        <v>-20491</v>
+        <v>-6099</v>
       </c>
       <c r="R7" s="18" t="n">
         <f aca="false">Q7*R8/Q8</f>
@@ -7815,7 +7815,7 @@
       <c r="P8" s="21"/>
       <c r="Q8" s="17" t="n">
         <f aca="false">C7</f>
-        <v>20491</v>
+        <v>6099</v>
       </c>
       <c r="R8" s="22" t="n">
         <v>1</v>
@@ -7827,7 +7827,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">C7-C8</f>
-        <v>14600.5</v>
+        <v>208.5</v>
       </c>
       <c r="D9" s="24" t="n">
         <f aca="false">D7-D8</f>
@@ -7835,47 +7835,47 @@
       </c>
       <c r="E9" s="25" t="n">
         <f aca="false">E7-E8</f>
-        <v>18174.64</v>
+        <v>-427.36</v>
       </c>
       <c r="F9" s="26" t="n">
         <f aca="false">F7-F8</f>
-        <v>12951.59</v>
+        <v>-1162.41</v>
       </c>
       <c r="G9" s="25" t="n">
         <f aca="false">G7-G8</f>
-        <v>17592.2</v>
+        <v>100.2</v>
       </c>
       <c r="H9" s="26" t="n">
         <f aca="false">H7-H8</f>
-        <v>17040.93</v>
+        <v>1250.93</v>
       </c>
       <c r="I9" s="25" t="n">
         <f aca="false">I7-I8</f>
-        <v>19581.14</v>
+        <v>16.1400000000003</v>
       </c>
       <c r="J9" s="26" t="n">
         <f aca="false">J7-J8</f>
-        <v>25229.63</v>
+        <v>4618.63</v>
       </c>
       <c r="K9" s="25" t="n">
         <f aca="false">K7-K8</f>
-        <v>22377.04</v>
+        <v>4458.04</v>
       </c>
       <c r="L9" s="25" t="n">
         <f aca="false">L7-L8</f>
-        <v>19840.93</v>
+        <v>2425.93</v>
       </c>
       <c r="M9" s="26" t="n">
         <f aca="false">M7-M8</f>
-        <v>16130.71</v>
+        <v>3279.71</v>
       </c>
       <c r="N9" s="25" t="n">
         <f aca="false">N7-N8</f>
-        <v>17679.05</v>
+        <v>1848.05</v>
       </c>
       <c r="O9" s="25" t="n">
         <f aca="false">O7-O8</f>
-        <v>201198.36</v>
+        <v>16616.36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7884,7 +7884,7 @@
       </c>
       <c r="C10" s="27" t="n">
         <f aca="false">C9+C6</f>
-        <v>14600.5</v>
+        <v>208.5</v>
       </c>
       <c r="D10" s="28" t="n">
         <f aca="false">D9+D6</f>
@@ -7892,47 +7892,47 @@
       </c>
       <c r="E10" s="29" t="n">
         <f aca="false">E9+E6</f>
-        <v>18174.64</v>
+        <v>-427.36</v>
       </c>
       <c r="F10" s="30" t="n">
         <f aca="false">F9+F6</f>
-        <v>12951.59</v>
+        <v>-1162.41</v>
       </c>
       <c r="G10" s="29" t="n">
         <f aca="false">G9+G6</f>
-        <v>17592.2</v>
+        <v>100.2</v>
       </c>
       <c r="H10" s="30" t="n">
         <f aca="false">H9+H6</f>
-        <v>17040.93</v>
+        <v>1250.93</v>
       </c>
       <c r="I10" s="29" t="n">
         <f aca="false">I9+I6</f>
-        <v>19581.14</v>
+        <v>16.1400000000003</v>
       </c>
       <c r="J10" s="30" t="n">
         <f aca="false">J9+J6</f>
-        <v>25229.63</v>
+        <v>4618.63</v>
       </c>
       <c r="K10" s="29" t="n">
         <f aca="false">K9+K6</f>
-        <v>22377.04</v>
+        <v>4458.04</v>
       </c>
       <c r="L10" s="29" t="n">
         <f aca="false">L9+L6</f>
-        <v>19840.93</v>
+        <v>2425.93</v>
       </c>
       <c r="M10" s="30" t="n">
         <f aca="false">M9+M6</f>
-        <v>16130.71</v>
+        <v>3279.71</v>
       </c>
       <c r="N10" s="29" t="n">
         <f aca="false">N9+N6</f>
-        <v>17679.05</v>
+        <v>1848.05</v>
       </c>
       <c r="O10" s="29" t="n">
         <f aca="false">O9+O6</f>
-        <v>201198.36</v>
+        <v>16616.36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7941,7 +7941,7 @@
       </c>
       <c r="C11" s="31" t="n">
         <f aca="false">C9*100%/C7</f>
-        <v>0.712532331267386</v>
+        <v>0.0341859321200197</v>
       </c>
       <c r="D11" s="32" t="e">
         <f aca="false">D9*100%/D7</f>
@@ -7949,47 +7949,47 @@
       </c>
       <c r="E11" s="33" t="n">
         <f aca="false">E9*100%/E7</f>
-        <v>0.733491079078564</v>
+        <v>-0.0691938662007975</v>
       </c>
       <c r="F11" s="32" t="n">
         <f aca="false">F9*100%/F7</f>
-        <v>0.683415772882647</v>
+        <v>-0.240303394897111</v>
       </c>
       <c r="G11" s="33" t="n">
         <f aca="false">G9*100%/G7</f>
-        <v>0.741885300067516</v>
+        <v>0.0161071754090692</v>
       </c>
       <c r="H11" s="32" t="n">
         <f aca="false">H9*100%/H7</f>
-        <v>0.848131524881149</v>
+        <v>0.290757079901077</v>
       </c>
       <c r="I11" s="33" t="n">
         <f aca="false">I9*100%/I7</f>
-        <v>0.784515888126054</v>
+        <v>0.00299192513884467</v>
       </c>
       <c r="J11" s="32" t="n">
         <f aca="false">J9*100%/J7</f>
-        <v>0.859532656757991</v>
+        <v>0.528342787983614</v>
       </c>
       <c r="K11" s="33" t="n">
         <f aca="false">K9*100%/K7</f>
-        <v>0.861184681969919</v>
+        <v>0.552762423403786</v>
       </c>
       <c r="L11" s="33" t="n">
         <f aca="false">L9*100%/L7</f>
-        <v>0.862005999002483</v>
+        <v>0.433034758021906</v>
       </c>
       <c r="M11" s="32" t="n">
         <f aca="false">M9*100%/M7</f>
-        <v>0.837170064157724</v>
+        <v>0.511085935479045</v>
       </c>
       <c r="N11" s="33" t="n">
         <f aca="false">N9*100%/N7</f>
-        <v>0.837229247390858</v>
+        <v>0.349669072153245</v>
       </c>
       <c r="O11" s="33" t="n">
         <f aca="false">O9*100%/O7</f>
-        <v>0.799283531021889</v>
+        <v>0.247483109896891</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8166,7 +8166,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8264,55 +8264,55 @@
       </c>
       <c r="B6" s="55" t="n">
         <f aca="false">SUM(B7:B9)</f>
-        <v>20491</v>
+        <v>6099</v>
       </c>
       <c r="C6" s="55" t="n">
         <f aca="false">SUM(C7:C9)</f>
-        <v>21280.56</v>
+        <v>7368.56</v>
       </c>
       <c r="D6" s="55" t="n">
         <f aca="false">SUM(D7:D9)</f>
-        <v>24778.27</v>
+        <v>6176.27</v>
       </c>
       <c r="E6" s="55" t="n">
         <f aca="false">SUM(E7:E9)</f>
-        <v>18951.26</v>
+        <v>4837.26</v>
       </c>
       <c r="F6" s="55" t="n">
         <f aca="false">SUM(F7:F9)</f>
-        <v>23712.83</v>
+        <v>6220.83</v>
       </c>
       <c r="G6" s="55" t="n">
         <f aca="false">SUM(G7:G9)</f>
-        <v>20092.32</v>
+        <v>4302.32</v>
       </c>
       <c r="H6" s="55" t="n">
         <f aca="false">SUM(H7:H9)</f>
-        <v>24959.52</v>
+        <v>5394.52</v>
       </c>
       <c r="I6" s="55" t="n">
         <f aca="false">SUM(I7:I9)</f>
-        <v>29352.73</v>
+        <v>8741.73</v>
       </c>
       <c r="J6" s="55" t="n">
         <f aca="false">SUM(J7:J9)</f>
-        <v>25984.02</v>
+        <v>8065.02</v>
       </c>
       <c r="K6" s="55" t="n">
         <f aca="false">SUM(K7:K9)</f>
-        <v>23017.16</v>
+        <v>5602.16</v>
       </c>
       <c r="L6" s="55" t="n">
         <f aca="false">SUM(L7:L9)</f>
-        <v>19268.14</v>
+        <v>6417.14</v>
       </c>
       <c r="M6" s="55" t="n">
         <f aca="false">SUM(M7:M9)</f>
-        <v>21116.14</v>
+        <v>5285.14</v>
       </c>
       <c r="N6" s="13" t="n">
         <f aca="false">SUM(B6:M6)</f>
-        <v>273003.95</v>
+        <v>74509.95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8329,7 +8329,7 @@
         <v>1420.37</v>
       </c>
       <c r="E7" s="11" t="n">
-        <v>957.83</v>
+        <v>1957.83</v>
       </c>
       <c r="F7" s="11" t="n">
         <v>2343.9</v>
@@ -8357,7 +8357,7 @@
       </c>
       <c r="N7" s="13" t="n">
         <f aca="false">SUM(B7:M7)</f>
-        <v>26588.67</v>
+        <v>27588.67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8365,44 +8365,44 @@
         <v>27</v>
       </c>
       <c r="B8" s="11" t="n">
-        <v>16324</v>
+        <v>1932</v>
       </c>
       <c r="C8" s="11" t="n">
-        <v>15457.76</v>
+        <v>1545.76</v>
       </c>
       <c r="D8" s="11" t="n">
-        <v>21557.9</v>
+        <v>2955.9</v>
       </c>
       <c r="E8" s="11" t="n">
-        <v>16793.43</v>
+        <v>1679.43</v>
       </c>
       <c r="F8" s="11" t="n">
-        <v>20768.93</v>
+        <v>3276.93</v>
       </c>
       <c r="G8" s="11" t="n">
-        <v>17544.82</v>
+        <v>1754.82</v>
       </c>
       <c r="H8" s="11" t="n">
-        <v>21738.79</v>
+        <v>2173.79</v>
       </c>
       <c r="I8" s="11" t="n">
-        <v>22901.43</v>
+        <v>2290.43</v>
       </c>
       <c r="J8" s="11" t="n">
-        <v>19910.21</v>
+        <v>1991.21</v>
       </c>
       <c r="K8" s="11" t="n">
-        <v>19349.74</v>
+        <v>1934.74</v>
       </c>
       <c r="L8" s="11" t="n">
-        <v>14278.85</v>
+        <v>1427.85</v>
       </c>
       <c r="M8" s="11" t="n">
-        <v>17589.42</v>
+        <v>1758.42</v>
       </c>
       <c r="N8" s="13" t="n">
         <f aca="false">SUM(B8:M8)</f>
-        <v>224215.28</v>
+        <v>24721.28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9190,55 +9190,55 @@
       </c>
       <c r="B26" s="55" t="n">
         <f aca="false">B6-B10</f>
-        <v>14600.5</v>
+        <v>208.5</v>
       </c>
       <c r="C26" s="55" t="n">
         <f aca="false">C6-C10</f>
-        <v>15422.35</v>
+        <v>1510.35</v>
       </c>
       <c r="D26" s="55" t="n">
         <f aca="false">D6-D10</f>
-        <v>18174.64</v>
+        <v>-427.36</v>
       </c>
       <c r="E26" s="55" t="n">
         <f aca="false">E6-E10</f>
-        <v>12951.59</v>
+        <v>-1162.41</v>
       </c>
       <c r="F26" s="55" t="n">
         <f aca="false">F6-F10</f>
-        <v>17592.2</v>
+        <v>100.2</v>
       </c>
       <c r="G26" s="55" t="n">
         <f aca="false">G6-G10</f>
-        <v>17040.93</v>
+        <v>1250.93</v>
       </c>
       <c r="H26" s="55" t="n">
         <f aca="false">H6-H10</f>
-        <v>19581.14</v>
+        <v>16.1400000000003</v>
       </c>
       <c r="I26" s="55" t="n">
         <f aca="false">I6-I10</f>
-        <v>25229.63</v>
+        <v>4618.63</v>
       </c>
       <c r="J26" s="55" t="n">
         <f aca="false">J6-J10</f>
-        <v>22377.04</v>
+        <v>4458.04</v>
       </c>
       <c r="K26" s="55" t="n">
         <f aca="false">K6-K10</f>
-        <v>19840.93</v>
+        <v>2425.93</v>
       </c>
       <c r="L26" s="55" t="n">
         <f aca="false">L6-L10</f>
-        <v>16130.71</v>
+        <v>3279.71</v>
       </c>
       <c r="M26" s="55" t="n">
         <f aca="false">M6-M10</f>
-        <v>17679.05</v>
+        <v>1848.05</v>
       </c>
       <c r="N26" s="55" t="n">
         <f aca="false">N6-N10</f>
-        <v>216620.71</v>
+        <v>18126.71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -9356,55 +9356,55 @@
       </c>
       <c r="C7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!B6</f>
-        <v>20491</v>
+        <v>6099</v>
       </c>
       <c r="D7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!C6</f>
-        <v>21280.56</v>
+        <v>7368.56</v>
       </c>
       <c r="E7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!D6</f>
-        <v>24778.27</v>
+        <v>6176.27</v>
       </c>
       <c r="F7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!E6</f>
-        <v>18951.26</v>
+        <v>4837.26</v>
       </c>
       <c r="G7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!F6</f>
-        <v>23712.83</v>
+        <v>6220.83</v>
       </c>
       <c r="H7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!G6</f>
-        <v>20092.32</v>
+        <v>4302.32</v>
       </c>
       <c r="I7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!H6</f>
-        <v>24959.52</v>
+        <v>5394.52</v>
       </c>
       <c r="J7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!I6</f>
-        <v>29352.73</v>
+        <v>8741.73</v>
       </c>
       <c r="K7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!J6</f>
-        <v>25984.02</v>
+        <v>8065.02</v>
       </c>
       <c r="L7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!K6</f>
-        <v>23017.16</v>
+        <v>5602.16</v>
       </c>
       <c r="M7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!L6</f>
-        <v>19268.14</v>
+        <v>6417.14</v>
       </c>
       <c r="N7" s="15" t="n">
         <f aca="false">'LIVRO CAIXA'!M6</f>
-        <v>21116.14</v>
+        <v>5285.14</v>
       </c>
       <c r="O7" s="16" t="n">
         <f aca="false">SUM(C7:N7)</f>
-        <v>273003.95</v>
+        <v>74509.95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9413,7 +9413,7 @@
       </c>
       <c r="C8" s="63" t="n">
         <f aca="false">(C7*100%/C6)-100%</f>
-        <v>0.184126430099499</v>
+        <v>-0.647553213743749</v>
       </c>
       <c r="D8" s="64" t="str">
         <f aca="false">IFERROR((D7*100%)/D6,"%")</f>
@@ -9453,15 +9453,15 @@
       </c>
       <c r="M8" s="65" t="n">
         <f aca="false">IFERROR((M7*100%)/M6,"%")</f>
-        <v>1.11346024268495</v>
+        <v>0.37083134447556</v>
       </c>
       <c r="N8" s="65" t="n">
         <f aca="false">IFERROR((N7*100%)/N6,"%")</f>
-        <v>1.2202517922835</v>
+        <v>0.305415741582942</v>
       </c>
       <c r="O8" s="65" t="n">
         <f aca="false">(O7*100%/O6)-100%</f>
-        <v>4.25875087789049</v>
+        <v>0.435251266416022</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9773,7 +9773,7 @@
       </c>
       <c r="C19" s="15" t="n">
         <f aca="false">C7-C13</f>
-        <v>14600.5</v>
+        <v>208.5</v>
       </c>
       <c r="D19" s="15" t="str">
         <f aca="false">'LIVRO CAIXA'!C25</f>
@@ -9821,7 +9821,7 @@
       </c>
       <c r="O19" s="16" t="n">
         <f aca="false">SUM(C19:N19)</f>
-        <v>22819.5</v>
+        <v>8427.5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9830,7 +9830,7 @@
       </c>
       <c r="C20" s="63" t="n">
         <f aca="false">(C19*100%/C18)-100%</f>
-        <v>0.489126687704111</v>
+        <v>-0.978734775220965</v>
       </c>
       <c r="D20" s="64" t="str">
         <f aca="false">IFERROR((D19*100%)/D18,"%")</f>
@@ -9878,7 +9878,7 @@
       </c>
       <c r="O20" s="65" t="n">
         <f aca="false">(O19*100%/O18)-100%</f>
-        <v>1.32739470908969</v>
+        <v>-0.14046675383539</v>
       </c>
     </row>
   </sheetData>
@@ -9977,7 +9977,7 @@
     <row r="5" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="73" t="n">
         <f aca="false">'FLUXO DE CAIXA'!M7</f>
-        <v>19268.14</v>
+        <v>6417.14</v>
       </c>
       <c r="B5" s="73"/>
       <c r="D5" s="73" t="n">
@@ -9987,7 +9987,7 @@
       <c r="E5" s="73"/>
       <c r="G5" s="73" t="n">
         <f aca="false">'LIVRO CAIXA'!L26</f>
-        <v>16130.71</v>
+        <v>3279.71</v>
       </c>
       <c r="H5" s="73"/>
       <c r="J5" s="74" t="s">
@@ -10005,7 +10005,7 @@
       </c>
       <c r="B6" s="77" t="n">
         <f aca="false">META!C8</f>
-        <v>0.184126430099499</v>
+        <v>-0.647553213743749</v>
       </c>
       <c r="D6" s="78" t="s">
         <v>65</v>
@@ -10019,7 +10019,7 @@
       </c>
       <c r="H6" s="77" t="n">
         <f aca="false">META!C20</f>
-        <v>0.489126687704111</v>
+        <v>-0.978734775220965</v>
       </c>
       <c r="J6" s="74"/>
       <c r="K6" s="74"/>
@@ -10187,7 +10187,7 @@
       </c>
       <c r="B23" s="18" t="n">
         <f aca="false">A23*$B$27/$A$27</f>
-        <v>0.36654578205481</v>
+        <v>0.503640498019314</v>
       </c>
       <c r="C23" s="88"/>
       <c r="J23" s="86"/>
@@ -10200,11 +10200,11 @@
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="90" t="n">
         <f aca="false">META!M7</f>
-        <v>19268.14</v>
+        <v>6417.14</v>
       </c>
       <c r="B24" s="18" t="n">
         <f aca="false">A24*$B$27/$A$27</f>
-        <v>0.408134155441894</v>
+        <v>0.186765683012843</v>
       </c>
       <c r="C24" s="88"/>
       <c r="D24" s="70"/>
@@ -10222,7 +10222,7 @@
       </c>
       <c r="B25" s="18" t="n">
         <f aca="false">A25*$B$27/$A$27</f>
-        <v>0.158863604157651</v>
+        <v>0.218281449773002</v>
       </c>
       <c r="C25" s="88"/>
       <c r="D25" s="70"/>
@@ -10240,7 +10240,7 @@
       </c>
       <c r="B26" s="18" t="n">
         <f aca="false">A26*$B$27/$A$27</f>
-        <v>0.0664564583456453</v>
+        <v>0.0913123691948412</v>
       </c>
       <c r="C26" s="88"/>
       <c r="D26" s="70"/>
@@ -10254,7 +10254,7 @@
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="91" t="n">
         <f aca="false">SUM(A23:A26)</f>
-        <v>47210.31</v>
+        <v>34359.31</v>
       </c>
       <c r="B27" s="22" t="n">
         <v>1</v>
@@ -11895,19 +11895,19 @@
       </c>
       <c r="C4" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!L26</f>
-        <v>16130.71</v>
+        <v>3279.71</v>
       </c>
       <c r="D4" s="177" t="n">
         <f aca="false">'FLUXO DE CAIXA'!M11</f>
-        <v>0.837170064157724</v>
+        <v>0.511085935479045</v>
       </c>
       <c r="E4" s="178" t="str">
         <f aca="false">IF(D4&gt;0,"↑","↓")&amp;" "&amp;TEXT(D4,"0%")</f>
-        <v>↑ 84%</v>
+        <v>↑ 51%</v>
       </c>
       <c r="F4" s="179" t="n">
         <f aca="false">'FLUXO DE CAIXA'!L7</f>
-        <v>23017.16</v>
+        <v>5602.16</v>
       </c>
       <c r="H4" s="41" t="s">
         <v>138</v>
@@ -11922,15 +11922,15 @@
       </c>
       <c r="C5" s="180" t="n">
         <f aca="false">'LIVRO CAIXA'!L6-'LIVRO CAIXA'!K6</f>
-        <v>-3749.02</v>
+        <v>814.98</v>
       </c>
       <c r="D5" s="181" t="n">
         <f aca="false">('LIVRO CAIXA'!L6-'LIVRO CAIXA'!K6*100%)/'LIVRO CAIXA'!L6</f>
-        <v>-0.194570934194998</v>
+        <v>0.127000501781167</v>
       </c>
       <c r="E5" s="175" t="str">
         <f aca="false">IF(D5&gt;0,"↑","↓")&amp;" "&amp;TEXT(D5,"0%")</f>
-        <v>↓ -19%</v>
+        <v>↑ 13%</v>
       </c>
       <c r="H5" s="41" t="n">
         <v>104</v>
@@ -11945,15 +11945,15 @@
       </c>
       <c r="C6" s="179" t="n">
         <f aca="false">META!M7-META!M6</f>
-        <v>1963.4</v>
+        <v>-10887.6</v>
       </c>
       <c r="D6" s="182" t="n">
         <f aca="false">META!C8</f>
-        <v>0.184126430099499</v>
+        <v>-0.647553213743749</v>
       </c>
       <c r="E6" s="175" t="str">
         <f aca="false">IF(D6&gt;0,"↑","↓")&amp;" "&amp;TEXT(D6,"0,00%")</f>
-        <v>↑ 18,41%</v>
+        <v>↓ -64,76%</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12325,7 +12325,7 @@
       </c>
       <c r="C41" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!B6</f>
-        <v>20491</v>
+        <v>6099</v>
       </c>
       <c r="D41" s="176" t="n">
         <v>0</v>
@@ -12344,11 +12344,11 @@
       </c>
       <c r="C42" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!C6</f>
-        <v>21280.56</v>
+        <v>7368.56</v>
       </c>
       <c r="D42" s="176" t="n">
         <f aca="false">C41</f>
-        <v>20491</v>
+        <v>6099</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12357,11 +12357,11 @@
       </c>
       <c r="C43" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!D6</f>
-        <v>24778.27</v>
+        <v>6176.27</v>
       </c>
       <c r="D43" s="176" t="n">
         <f aca="false">C42</f>
-        <v>21280.56</v>
+        <v>7368.56</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12370,11 +12370,11 @@
       </c>
       <c r="C44" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!E6</f>
-        <v>18951.26</v>
+        <v>4837.26</v>
       </c>
       <c r="D44" s="176" t="n">
         <f aca="false">C43</f>
-        <v>24778.27</v>
+        <v>6176.27</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12383,11 +12383,11 @@
       </c>
       <c r="C45" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!F6</f>
-        <v>23712.83</v>
+        <v>6220.83</v>
       </c>
       <c r="D45" s="176" t="n">
         <f aca="false">C44</f>
-        <v>18951.26</v>
+        <v>4837.26</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12396,11 +12396,11 @@
       </c>
       <c r="C46" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!G6</f>
-        <v>20092.32</v>
+        <v>4302.32</v>
       </c>
       <c r="D46" s="176" t="n">
         <f aca="false">C45</f>
-        <v>23712.83</v>
+        <v>6220.83</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12409,11 +12409,11 @@
       </c>
       <c r="C47" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!H6</f>
-        <v>24959.52</v>
+        <v>5394.52</v>
       </c>
       <c r="D47" s="176" t="n">
         <f aca="false">C46</f>
-        <v>20092.32</v>
+        <v>4302.32</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12422,11 +12422,11 @@
       </c>
       <c r="C48" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!I6</f>
-        <v>29352.73</v>
+        <v>8741.73</v>
       </c>
       <c r="D48" s="176" t="n">
         <f aca="false">C47</f>
-        <v>24959.52</v>
+        <v>5394.52</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12435,11 +12435,11 @@
       </c>
       <c r="C49" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!J6</f>
-        <v>25984.02</v>
+        <v>8065.02</v>
       </c>
       <c r="D49" s="176" t="n">
         <f aca="false">C48</f>
-        <v>29352.73</v>
+        <v>8741.73</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12448,11 +12448,11 @@
       </c>
       <c r="C50" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!K6</f>
-        <v>23017.16</v>
+        <v>5602.16</v>
       </c>
       <c r="D50" s="176" t="n">
         <f aca="false">C49</f>
-        <v>25984.02</v>
+        <v>8065.02</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12461,11 +12461,11 @@
       </c>
       <c r="C51" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!L6</f>
-        <v>19268.14</v>
+        <v>6417.14</v>
       </c>
       <c r="D51" s="176" t="n">
         <f aca="false">C50</f>
-        <v>23017.16</v>
+        <v>5602.16</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12474,18 +12474,18 @@
       </c>
       <c r="C52" s="176" t="n">
         <f aca="false">'LIVRO CAIXA'!M6</f>
-        <v>21116.14</v>
+        <v>5285.14</v>
       </c>
       <c r="D52" s="176" t="n">
         <f aca="false">C51</f>
-        <v>19268.14</v>
+        <v>6417.14</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="184"/>
       <c r="D53" s="184" t="n">
         <f aca="false">'FLUXO DE CAIXA'!C7</f>
-        <v>20491</v>
+        <v>6099</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>